<commit_message>
added responses for questionnaire
</commit_message>
<xml_diff>
--- a/Responses_questionnaire_for_editors.xlsx
+++ b/Responses_questionnaire_for_editors.xlsx
@@ -70,28 +70,34 @@
     <t>Computational Intelligence</t>
   </si>
   <si>
+    <t>PeerJ, JOT</t>
+  </si>
+  <si>
+    <t>Frames with long scrollable content are not very user friendly. A system that is read-only is of limited usefulness.</t>
+  </si>
+  <si>
     <t>Data Science, IJSWS</t>
   </si>
   <si>
-    <t>PeerJ, JOT</t>
+    <t>Peer J in Computer Science</t>
   </si>
   <si>
     <t>Data Science</t>
   </si>
   <si>
-    <t>Frames with long scrollable content are not very user friendly. A system that is read-only is of limited usefulness.</t>
+    <t>I think attempts to create such taxonomies induce a tyranny of numbers and a reduction in nuanced evaluation.</t>
   </si>
   <si>
     <t xml:space="preserve">On the "reviewer-oriented" view, each "row" of data needs to be labeled. I know there is a legend, but it is very awkward to refer to it. Also, would the reviewers have to answer a question for each of these data points? This sounds enormously cumbersome. Overall, I think it is key to make life easier for reviewer, more than for editors. I also think there is simply too much information displayed on the graph. E.g., why do I need to know there are 7 comments by R3 at the article level, and 8 at the section level?  </t>
   </si>
   <si>
+    <t>PeerJ, Science of Computer Programming</t>
+  </si>
+  <si>
     <t>Journal of Data Science</t>
   </si>
   <si>
-    <t>Peer J in Computer Science</t>
-  </si>
-  <si>
-    <t>I think attempts to create such taxonomies induce a tyranny of numbers and a reduction in nuanced evaluation.</t>
+    <t>Peerj</t>
   </si>
   <si>
     <t>BMC Bioinformatics, BMC Medical Informatics and Decision Making</t>
@@ -100,7 +106,7 @@
     <t>I find the "Reviewer view" very cluttered and therefore a bit difficult to discern patterns out of. I'm wondering whether it might be better to either allow the editor to dynamically select which aspect they are interested in, and only focus on those, or somehow group the different aspects together across the reviewers (e.g. group by Level/Aspect/Positivity/etc. rather than by Reviewer) so that broader patterns related to each of those levels can be discerned.</t>
   </si>
   <si>
-    <t>PeerJ, Science of Computer Programming</t>
+    <t>many</t>
   </si>
   <si>
     <t>PeerJ Computer Science, Data Science (IOS Press)</t>
@@ -109,7 +115,10 @@
     <t>There are too many colours in the interface, while there are 5 different dimensions. I would strongly suggest to use other techniques – different shapes, sizes, etc. – so as to carry the required information for the dimension. In principle, you should use only one technique per dimension. E.g. use colours for positivity/negativity comments, use shapes for article level comments, use sizes for impact, etc.</t>
   </si>
   <si>
-    <t>Peerj</t>
+    <t>JAAMAS, Adv. Complex Systems, TR-C (guest ed.)</t>
+  </si>
+  <si>
+    <t>I like the idea but I am extremely concerned that it will turn the process into a quantitative process only, whereas I still believe in qualitative analysis. However, perhaps it would be very useful to filter out for conferences (or even journals) that receive a lot of submissions. In this case, the initial reviewing could be a simplyfied one with an output given by such tool. Other than that I myself would use it just as an auxiliatory tool.</t>
   </si>
   <si>
     <t xml:space="preserve">The first time this question was asked ""What is the number of positive comments and the number of negative comments per section of the article?"" the responses provided do not seem to make sense.  It is not possible to answer "what is the number.." with a reply of very important or not important.  It should be answered with a quantitative response, so this was not really clear to me.
@@ -119,15 +128,6 @@
 </t>
   </si>
   <si>
-    <t>many</t>
-  </si>
-  <si>
-    <t>JAAMAS, Adv. Complex Systems, TR-C (guest ed.)</t>
-  </si>
-  <si>
-    <t>I like the idea but I am extremely concerned that it will turn the process into a quantitative process only, whereas I still believe in qualitative analysis. However, perhaps it would be very useful to filter out for conferences (or even journals) that receive a lot of submissions. In this case, the initial reviewing could be a simplyfied one with an output given by such tool. Other than that I myself would use it just as an auxiliatory tool.</t>
-  </si>
-  <si>
     <t>PEEJ</t>
   </si>
   <si>
@@ -140,22 +140,22 @@
     <t>when can I start using the tool!</t>
   </si>
   <si>
+    <t>PeerJ</t>
+  </si>
+  <si>
+    <t>Frontiers, PlosOne, PeerJ</t>
+  </si>
+  <si>
+    <t>I find the presentations of these interfaces disturbing because of the two many colours. I prefer to read and think quietly at referees' suggestions.</t>
+  </si>
+  <si>
     <t>Data science journal</t>
   </si>
   <si>
-    <t>PeerJ</t>
+    <t>SoSyM, PeerJ</t>
   </si>
   <si>
     <t>Data Science Journal</t>
-  </si>
-  <si>
-    <t>Frontiers, PlosOne, PeerJ</t>
-  </si>
-  <si>
-    <t>I find the presentations of these interfaces disturbing because of the two many colours. I prefer to read and think quietly at referees' suggestions.</t>
-  </si>
-  <si>
-    <t>SoSyM, PeerJ</t>
   </si>
   <si>
     <t>Scientific report, PeerJ</t>
@@ -557,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -587,7 +587,13 @@
     <xf borderId="5" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="7" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -604,6 +610,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -623,8 +630,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="18" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -634,12 +645,10 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="9" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="15" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -946,11 +955,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1520510688"/>
-        <c:axId val="637710371"/>
+        <c:axId val="383632101"/>
+        <c:axId val="1561440771"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1520510688"/>
+        <c:axId val="383632101"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -995,10 +1004,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="637710371"/>
+        <c:crossAx val="1561440771"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="637710371"/>
+        <c:axId val="1561440771"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1076,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1520510688"/>
+        <c:crossAx val="383632101"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -1357,11 +1366,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="1937635491"/>
-        <c:axId val="889567430"/>
+        <c:axId val="1539638754"/>
+        <c:axId val="1665339004"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1937635491"/>
+        <c:axId val="1539638754"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1406,10 +1415,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="889567430"/>
+        <c:crossAx val="1665339004"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="889567430"/>
+        <c:axId val="1665339004"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1478,7 +1487,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1937635491"/>
+        <c:crossAx val="1539638754"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -1813,52 +1822,52 @@
       <c r="Q1" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="T1" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="17">
         <v>1.0</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="18">
         <f>SUM(Data_Science_Journal!B$24, PeerJ_in_Computer_Science_Journ!B$36, Semantic_Web_Journal!B$17)</f>
         <v>5</v>
       </c>
-      <c r="D2" s="15">
-        <v>2.0</v>
-      </c>
-      <c r="E2" s="16">
+      <c r="D2" s="17">
+        <v>2.0</v>
+      </c>
+      <c r="E2" s="18">
         <f>SUM(Data_Science_Journal!B$25, PeerJ_in_Computer_Science_Journ!B$37, Semantic_Web_Journal!B$18)</f>
         <v>10</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="17">
         <v>3.0</v>
       </c>
       <c r="G2" s="6">
         <f>SUM(Data_Science_Journal!B$26, PeerJ_in_Computer_Science_Journ!B$38, Semantic_Web_Journal!B$19)</f>
         <v>10</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="17">
         <v>4.0</v>
       </c>
       <c r="I2" s="6">
         <f>SUM(Data_Science_Journal!B$27, PeerJ_in_Computer_Science_Journ!B$39, Semantic_Web_Journal!B$20)</f>
         <v>7</v>
       </c>
-      <c r="J2" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K2" s="17">
+      <c r="J2" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K2" s="19">
         <f>SUM(Data_Science_Journal!B$28, PeerJ_in_Computer_Science_Journ!B$40, Semantic_Web_Journal!B$21)</f>
         <v>10</v>
       </c>
@@ -1866,7 +1875,7 @@
         <f t="shared" ref="L2:L8" si="1">(B2*C2+D2*E2+F2*G2+H2*I2+J2*K2)/(C2+E2+G2+I2+K2)</f>
         <v>3.166666667</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="20">
         <f>MEDIAN(Data_Science_Journal!B$2:B$22,PeerJ_in_Computer_Science_Journ!B$2:B$33,Semantic_Web_Journal!B$2:B$15)</f>
         <v>3</v>
       </c>
@@ -1874,7 +1883,7 @@
         <f>STDEV(Data_Science_Journal!B$2:B$22,PeerJ_in_Computer_Science_Journ!B$2:B$33,Semantic_Web_Journal!B$2:B$15)</f>
         <v>1.359997609</v>
       </c>
-      <c r="O2" s="19">
+      <c r="O2" s="21">
         <f t="shared" ref="O2:O8" si="2">C2+E2</f>
         <v>15</v>
       </c>
@@ -1886,55 +1895,55 @@
         <f t="shared" ref="Q2:Q8" si="4">O2+P2</f>
         <v>42</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="22">
         <f t="shared" ref="R2:R8" si="5">if(O2&lt;P2,BINOMDIST(O2,Q2,0.5,TRUE),BINOMDIST(P2,Q2,0.5,TRUE))*2</f>
         <v>0.08842954699</v>
       </c>
-      <c r="S2" s="1">
+      <c r="S2" s="22">
         <f t="shared" ref="S2:S8" si="6">BINOMDIST(P2,Q2,0.5,TRUE)</f>
         <v>0.978220739</v>
       </c>
-      <c r="T2" s="20">
+      <c r="T2" s="23">
         <f t="shared" ref="T2:T8" si="7">BINOMDIST(O2,Q2,0.5,TRUE)</f>
         <v>0.04421477349</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="17">
         <v>1.0</v>
       </c>
       <c r="C3" s="6">
         <f>SUM(Data_Science_Journal!C24, PeerJ_in_Computer_Science_Journ!C36, Semantic_Web_Journal!C17)</f>
         <v>11</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="17">
         <v>2.0</v>
       </c>
       <c r="E3" s="6">
         <f>SUM(Data_Science_Journal!C25, PeerJ_in_Computer_Science_Journ!C37, Semantic_Web_Journal!C18)</f>
         <v>13</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="17">
         <v>3.0</v>
       </c>
       <c r="G3" s="6">
         <f>SUM(Data_Science_Journal!C26, PeerJ_in_Computer_Science_Journ!C38, Semantic_Web_Journal!C19)</f>
         <v>11</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="17">
         <v>4.0</v>
       </c>
       <c r="I3" s="6">
         <f>SUM(Data_Science_Journal!C27, PeerJ_in_Computer_Science_Journ!C39, Semantic_Web_Journal!C20)</f>
         <v>6</v>
       </c>
-      <c r="J3" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K3" s="17">
+      <c r="J3" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K3" s="19">
         <f>SUM(Data_Science_Journal!C$28, PeerJ_in_Computer_Science_Journ!C$40, Semantic_Web_Journal!C$21)</f>
         <v>1</v>
       </c>
@@ -1942,7 +1951,7 @@
         <f t="shared" si="1"/>
         <v>2.357142857</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="20">
         <f>MEDIAN(Data_Science_Journal!C$2:C$22,PeerJ_in_Computer_Science_Journ!C$2:C$33,Semantic_Web_Journal!C$2:C$15)</f>
         <v>2</v>
       </c>
@@ -1950,7 +1959,7 @@
         <f>STDEV(Data_Science_Journal!C$2:C$22,PeerJ_in_Computer_Science_Journ!C$2:C$33,Semantic_Web_Journal!C$2:C$15)</f>
         <v>1.10036421</v>
       </c>
-      <c r="O3" s="19">
+      <c r="O3" s="21">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
@@ -1962,55 +1971,55 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="22">
         <f t="shared" si="5"/>
         <v>0.4407990673</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="22">
         <f t="shared" si="6"/>
         <v>0.2203995337</v>
       </c>
-      <c r="T3" s="20">
+      <c r="T3" s="23">
         <f t="shared" si="7"/>
         <v>0.8600218807</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="17">
         <v>1.0</v>
       </c>
       <c r="C4" s="6">
         <f>SUM(Data_Science_Journal!D24, PeerJ_in_Computer_Science_Journ!D36, Semantic_Web_Journal!D17)</f>
         <v>1</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="17">
         <v>2.0</v>
       </c>
       <c r="E4" s="6">
         <f>SUM(Data_Science_Journal!D25, PeerJ_in_Computer_Science_Journ!D37, Semantic_Web_Journal!D18)</f>
         <v>4</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="17">
         <v>3.0</v>
       </c>
       <c r="G4" s="6">
         <f>SUM(Data_Science_Journal!D26, PeerJ_in_Computer_Science_Journ!D38, Semantic_Web_Journal!D19)</f>
         <v>10</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="17">
         <v>4.0</v>
       </c>
       <c r="I4" s="6">
         <f>SUM(Data_Science_Journal!D27, PeerJ_in_Computer_Science_Journ!D39, Semantic_Web_Journal!D20)</f>
         <v>21</v>
       </c>
-      <c r="J4" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K4" s="17">
+      <c r="J4" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K4" s="19">
         <f>SUM(Data_Science_Journal!D$28, PeerJ_in_Computer_Science_Journ!D$40, Semantic_Web_Journal!D$21)</f>
         <v>6</v>
       </c>
@@ -2018,7 +2027,7 @@
         <f t="shared" si="1"/>
         <v>3.642857143</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="20">
         <f>MEDIAN(Data_Science_Journal!D$2:D$22,PeerJ_in_Computer_Science_Journ!D$2:D$33,Semantic_Web_Journal!D$2:D$15)</f>
         <v>4</v>
       </c>
@@ -2026,7 +2035,7 @@
         <f>STDEV(Data_Science_Journal!D$2:D$22,PeerJ_in_Computer_Science_Journ!D$2:D$33,Semantic_Web_Journal!D$2:D$15)</f>
         <v>0.9323829573</v>
       </c>
-      <c r="O4" s="19">
+      <c r="O4" s="21">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -2038,55 +2047,55 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="22">
         <f t="shared" si="5"/>
         <v>0.0000004433704817</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="22">
         <f t="shared" si="6"/>
         <v>0.9999999717</v>
       </c>
-      <c r="T4" s="20">
+      <c r="T4" s="23">
         <f t="shared" si="7"/>
         <v>0.0000002216852408</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="17">
         <v>1.0</v>
       </c>
       <c r="C5" s="6">
         <f>SUM(Data_Science_Journal!E24, PeerJ_in_Computer_Science_Journ!E36, Semantic_Web_Journal!E17)</f>
         <v>6</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="17">
         <v>2.0</v>
       </c>
       <c r="E5" s="6">
         <f>SUM(Data_Science_Journal!E25, PeerJ_in_Computer_Science_Journ!E37, Semantic_Web_Journal!E18)</f>
         <v>8</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="17">
         <v>3.0</v>
       </c>
       <c r="G5" s="6">
         <f>SUM(Data_Science_Journal!E26, PeerJ_in_Computer_Science_Journ!E38, Semantic_Web_Journal!E19)</f>
         <v>8</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="17">
         <v>4.0</v>
       </c>
       <c r="I5" s="6">
         <f>SUM(Data_Science_Journal!E27, PeerJ_in_Computer_Science_Journ!E39, Semantic_Web_Journal!E20)</f>
         <v>18</v>
       </c>
-      <c r="J5" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K5" s="17">
+      <c r="J5" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K5" s="19">
         <f>SUM(Data_Science_Journal!E$28, PeerJ_in_Computer_Science_Journ!E$40, Semantic_Web_Journal!E$21)</f>
         <v>2</v>
       </c>
@@ -2094,7 +2103,7 @@
         <f t="shared" si="1"/>
         <v>3.047619048</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="20">
         <f>MEDIAN(Data_Science_Journal!E$2:E$22,PeerJ_in_Computer_Science_Journ!E$2:E$33,Semantic_Web_Journal!E$2:E$15)</f>
         <v>3</v>
       </c>
@@ -2102,7 +2111,7 @@
         <f>STDEV(Data_Science_Journal!E$2:E$22,PeerJ_in_Computer_Science_Journ!E$2:E$33,Semantic_Web_Journal!E$2:E$15)</f>
         <v>1.188407029</v>
       </c>
-      <c r="O5" s="19">
+      <c r="O5" s="21">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
@@ -2114,55 +2123,55 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R5" s="1">
+      <c r="R5" s="22">
         <f t="shared" si="5"/>
         <v>0.04355852192</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="22">
         <f t="shared" si="6"/>
         <v>0.9902397636</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="23">
         <f t="shared" si="7"/>
         <v>0.02177926096</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="17">
         <v>1.0</v>
       </c>
       <c r="C6" s="6">
         <f>SUM(Data_Science_Journal!F24, PeerJ_in_Computer_Science_Journ!F36, Semantic_Web_Journal!F17)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="17">
         <v>2.0</v>
       </c>
       <c r="E6" s="6">
         <f>SUM(Data_Science_Journal!F25, PeerJ_in_Computer_Science_Journ!F37, Semantic_Web_Journal!F18)</f>
         <v>0</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="17">
         <v>3.0</v>
       </c>
       <c r="G6" s="6">
         <f>SUM(Data_Science_Journal!F26, PeerJ_in_Computer_Science_Journ!F38, Semantic_Web_Journal!F19)</f>
         <v>3</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="17">
         <v>4.0</v>
       </c>
       <c r="I6" s="6">
         <f>SUM(Data_Science_Journal!F27, PeerJ_in_Computer_Science_Journ!F39, Semantic_Web_Journal!F20)</f>
         <v>12</v>
       </c>
-      <c r="J6" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K6" s="17">
+      <c r="J6" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K6" s="19">
         <f>SUM(Data_Science_Journal!F$28, PeerJ_in_Computer_Science_Journ!F$40, Semantic_Web_Journal!F$21)</f>
         <v>27</v>
       </c>
@@ -2170,7 +2179,7 @@
         <f t="shared" si="1"/>
         <v>4.571428571</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="20">
         <f>MEDIAN(Data_Science_Journal!F$2:F$22,PeerJ_in_Computer_Science_Journ!F$2:F$33,Semantic_Web_Journal!F$2:F$15)</f>
         <v>5</v>
       </c>
@@ -2178,7 +2187,7 @@
         <f>STDEV(Data_Science_Journal!F$2:F$22,PeerJ_in_Computer_Science_Journ!F$2:F$33,Semantic_Web_Journal!F$2:F$15)</f>
         <v>0.6302480016</v>
       </c>
-      <c r="O6" s="19">
+      <c r="O6" s="21">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2190,55 +2199,55 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R6" s="1">
+      <c r="R6" s="22">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="22">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="T6" s="20">
+      <c r="T6" s="23">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="17">
         <v>1.0</v>
       </c>
       <c r="C7" s="6">
         <f>SUM(Data_Science_Journal!G24, PeerJ_in_Computer_Science_Journ!G36, Semantic_Web_Journal!G17)</f>
         <v>2</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="17">
         <v>2.0</v>
       </c>
       <c r="E7" s="6">
         <f>SUM(Data_Science_Journal!G25, PeerJ_in_Computer_Science_Journ!G37, Semantic_Web_Journal!G18)</f>
         <v>4</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="17">
         <v>3.0</v>
       </c>
       <c r="G7" s="6">
         <f>SUM(Data_Science_Journal!G26, PeerJ_in_Computer_Science_Journ!G38, Semantic_Web_Journal!G19)</f>
         <v>10</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="17">
         <v>4.0</v>
       </c>
       <c r="I7" s="6">
         <f>SUM(Data_Science_Journal!G27, PeerJ_in_Computer_Science_Journ!G39, Semantic_Web_Journal!G20)</f>
         <v>20</v>
       </c>
-      <c r="J7" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K7" s="17">
+      <c r="J7" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K7" s="19">
         <f>SUM(Data_Science_Journal!G$28, PeerJ_in_Computer_Science_Journ!G$40, Semantic_Web_Journal!G$21)</f>
         <v>6</v>
       </c>
@@ -2246,7 +2255,7 @@
         <f t="shared" si="1"/>
         <v>3.571428571</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="20">
         <f>MEDIAN(Data_Science_Journal!G$2:G$22,PeerJ_in_Computer_Science_Journ!G$2:G$33,Semantic_Web_Journal!G$2:G$15)</f>
         <v>4</v>
       </c>
@@ -2254,7 +2263,7 @@
         <f>STDEV(Data_Science_Journal!G$2:G$22,PeerJ_in_Computer_Science_Journ!G$2:G$33,Semantic_Web_Journal!G$2:G$15)</f>
         <v>1.01555841</v>
       </c>
-      <c r="O7" s="19">
+      <c r="O7" s="21">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -2266,91 +2275,91 @@
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7" s="22">
         <f t="shared" si="5"/>
         <v>0.000002828877768</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="22">
         <f t="shared" si="6"/>
         <v>0.9999997783</v>
       </c>
-      <c r="T7" s="20">
+      <c r="T7" s="23">
         <f t="shared" si="7"/>
         <v>0.000001414438884</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="25">
         <v>1.0</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="26">
         <f>SUM(Data_Science_Journal!H24, PeerJ_in_Computer_Science_Journ!H36, Semantic_Web_Journal!H17)</f>
         <v>6</v>
       </c>
-      <c r="D8" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="D8" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="26">
         <f>SUM(Data_Science_Journal!H25, PeerJ_in_Computer_Science_Journ!H37, Semantic_Web_Journal!H18)</f>
         <v>12</v>
       </c>
-      <c r="F8" s="22">
-        <v>3.0</v>
-      </c>
-      <c r="G8" s="23">
+      <c r="F8" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="26">
         <f>SUM(Data_Science_Journal!H26, PeerJ_in_Computer_Science_Journ!H38, Semantic_Web_Journal!H19)</f>
         <v>10</v>
       </c>
-      <c r="H8" s="22">
-        <v>4.0</v>
-      </c>
-      <c r="I8" s="23">
+      <c r="H8" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="I8" s="26">
         <f>SUM(Data_Science_Journal!H27, PeerJ_in_Computer_Science_Journ!H39, Semantic_Web_Journal!H20)</f>
         <v>13</v>
       </c>
-      <c r="J8" s="22">
-        <v>5.0</v>
-      </c>
-      <c r="K8" s="24">
+      <c r="J8" s="25">
+        <v>5.0</v>
+      </c>
+      <c r="K8" s="27">
         <f>SUM(Data_Science_Journal!H$28, PeerJ_in_Computer_Science_Journ!H$40, Semantic_Web_Journal!H$21)</f>
         <v>1</v>
       </c>
-      <c r="L8" s="25">
+      <c r="L8" s="28">
         <f t="shared" si="1"/>
         <v>2.785714286</v>
       </c>
-      <c r="M8" s="26">
+      <c r="M8" s="29">
         <f>MEDIAN(Data_Science_Journal!H$2:H$22,PeerJ_in_Computer_Science_Journ!H$2:H$33,Semantic_Web_Journal!H$2:H$15)</f>
         <v>3</v>
       </c>
-      <c r="N8" s="27">
+      <c r="N8" s="30">
         <f>STDEV(Data_Science_Journal!H$2:H$22,PeerJ_in_Computer_Science_Journ!H$2:H$33,Semantic_Web_Journal!H$2:H$15)</f>
         <v>1.116084495</v>
       </c>
-      <c r="O8" s="28">
+      <c r="O8" s="31">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="P8" s="25">
+      <c r="P8" s="28">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="Q8" s="25">
+      <c r="Q8" s="28">
         <f t="shared" si="4"/>
         <v>42</v>
       </c>
-      <c r="R8" s="25">
+      <c r="R8" s="32">
         <f t="shared" si="5"/>
         <v>0.4407990673</v>
       </c>
-      <c r="S8" s="25">
+      <c r="S8" s="32">
         <f t="shared" si="6"/>
         <v>0.8600218807</v>
       </c>
-      <c r="T8" s="29">
+      <c r="T8" s="33">
         <f t="shared" si="7"/>
         <v>0.2203995337</v>
       </c>
@@ -2406,46 +2415,46 @@
       <c r="S10" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="T10" s="34" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="17">
         <v>1.0</v>
       </c>
       <c r="C11" s="6">
         <f>SUM(Data_Science_Journal!I$24, PeerJ_in_Computer_Science_Journ!I$36, Semantic_Web_Journal!I$17)</f>
         <v>3</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="17">
         <v>2.0</v>
       </c>
       <c r="E11" s="6">
         <f>SUM(Data_Science_Journal!I$25, PeerJ_in_Computer_Science_Journ!I$37, Semantic_Web_Journal!I$18)</f>
         <v>6</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="17">
         <v>3.0</v>
       </c>
       <c r="G11" s="6">
         <f>SUM(Data_Science_Journal!I$26, PeerJ_in_Computer_Science_Journ!I$38, Semantic_Web_Journal!I$19)</f>
         <v>9</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="17">
         <v>4.0</v>
       </c>
       <c r="I11" s="6">
         <f>SUM(Data_Science_Journal!I$27, PeerJ_in_Computer_Science_Journ!I$39, Semantic_Web_Journal!I$20)</f>
         <v>16</v>
       </c>
-      <c r="J11" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K11" s="17">
+      <c r="J11" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K11" s="19">
         <f>SUM(Data_Science_Journal!I$28, PeerJ_in_Computer_Science_Journ!I$40, Semantic_Web_Journal!I$21)</f>
         <v>8</v>
       </c>
@@ -2453,7 +2462,7 @@
         <f t="shared" ref="L11:L17" si="8">(B11*C11+D11*E11+F11*G11+H11*I11+J11*K11)/(C11+E11+G11+I11+K11)</f>
         <v>3.476190476</v>
       </c>
-      <c r="M11" s="30">
+      <c r="M11" s="35">
         <f>MEDIAN(Data_Science_Journal!I$2:I$22,PeerJ_in_Computer_Science_Journ!I$2:I$33,Semantic_Web_Journal!I$2:I$15)</f>
         <v>4</v>
       </c>
@@ -2461,67 +2470,67 @@
         <f>STDEV(Data_Science_Journal!I$2:I$22,PeerJ_in_Computer_Science_Journ!I$2:I$33,Semantic_Web_Journal!I$2:I$15)</f>
         <v>1.173655853</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="36">
         <f t="shared" ref="O11:O17" si="9">C11+E11</f>
         <v>9</v>
       </c>
-      <c r="P11" s="32">
+      <c r="P11" s="37">
         <f t="shared" ref="P11:P17" si="10">G11+I11+K11</f>
         <v>33</v>
       </c>
-      <c r="Q11" s="32">
+      <c r="Q11" s="37">
         <f t="shared" ref="Q11:Q17" si="11">O11+P11</f>
         <v>42</v>
       </c>
-      <c r="R11" s="33">
+      <c r="R11" s="38">
         <f t="shared" ref="R11:R17" si="12">if(O11&lt;P11,BINOMDIST(O11,Q11,0.5,TRUE),BINOMDIST(P11,Q11,0.5,TRUE))*2</f>
         <v>0.0002715392343</v>
       </c>
-      <c r="S11" s="33">
+      <c r="S11" s="38">
         <f t="shared" ref="S11:S17" si="13">BINOMDIST(P11,Q11,0.5,TRUE)</f>
         <v>0.9999656144</v>
       </c>
-      <c r="T11" s="34">
+      <c r="T11" s="39">
         <f t="shared" ref="T11:T17" si="14">BINOMDIST(O11,Q11,0.5,TRUE)</f>
         <v>0.0001357696171</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="17">
         <v>1.0</v>
       </c>
       <c r="C12" s="6">
         <f>SUM(Data_Science_Journal!J$24, PeerJ_in_Computer_Science_Journ!J$36, Semantic_Web_Journal!J$17)</f>
         <v>1</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="17">
         <v>2.0</v>
       </c>
       <c r="E12" s="6">
         <f>SUM(Data_Science_Journal!J$25, PeerJ_in_Computer_Science_Journ!J$37, Semantic_Web_Journal!J$18)</f>
         <v>4</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="17">
         <v>3.0</v>
       </c>
       <c r="G12" s="6">
         <f>SUM(Data_Science_Journal!J$26, PeerJ_in_Computer_Science_Journ!J$38, Semantic_Web_Journal!J$19)</f>
         <v>8</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="17">
         <v>4.0</v>
       </c>
       <c r="I12" s="6">
         <f>SUM(Data_Science_Journal!J$27, PeerJ_in_Computer_Science_Journ!J$39, Semantic_Web_Journal!J$20)</f>
         <v>17</v>
       </c>
-      <c r="J12" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K12" s="17">
+      <c r="J12" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K12" s="19">
         <f>SUM(Data_Science_Journal!J$28, PeerJ_in_Computer_Science_Journ!J$40, Semantic_Web_Journal!J$21)</f>
         <v>12</v>
       </c>
@@ -2529,7 +2538,7 @@
         <f t="shared" si="8"/>
         <v>3.833333333</v>
       </c>
-      <c r="M12" s="35">
+      <c r="M12" s="40">
         <f>MEDIAN(Data_Science_Journal!J$2:J$22,PeerJ_in_Computer_Science_Journ!J$2:J$33,Semantic_Web_Journal!J$2:J$15)</f>
         <v>4</v>
       </c>
@@ -2537,7 +2546,7 @@
         <f>STDEV(Data_Science_Journal!J$2:J$22,PeerJ_in_Computer_Science_Journ!J$2:J$33,Semantic_Web_Journal!J$2:J$15)</f>
         <v>1.033975672</v>
       </c>
-      <c r="O12" s="19">
+      <c r="O12" s="21">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
@@ -2549,55 +2558,55 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R12" s="36">
+      <c r="R12" s="22">
         <f t="shared" si="12"/>
         <v>0.0000004433704817</v>
       </c>
-      <c r="S12" s="36">
+      <c r="S12" s="22">
         <f t="shared" si="13"/>
         <v>0.9999999717</v>
       </c>
-      <c r="T12" s="20">
+      <c r="T12" s="23">
         <f t="shared" si="14"/>
         <v>0.0000002216852408</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="17">
         <v>1.0</v>
       </c>
       <c r="C13" s="6">
         <f>SUM(Data_Science_Journal!K$24, PeerJ_in_Computer_Science_Journ!K$36, Semantic_Web_Journal!K$17)</f>
         <v>1</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="17">
         <v>2.0</v>
       </c>
       <c r="E13" s="6">
         <f>SUM(Data_Science_Journal!K$25, PeerJ_in_Computer_Science_Journ!K$37, Semantic_Web_Journal!K$18)</f>
         <v>8</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="17">
         <v>3.0</v>
       </c>
       <c r="G13" s="6">
         <f>SUM(Data_Science_Journal!K$26, PeerJ_in_Computer_Science_Journ!K$38, Semantic_Web_Journal!K$19)</f>
         <v>12</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="17">
         <v>4.0</v>
       </c>
       <c r="I13" s="6">
         <f>SUM(Data_Science_Journal!K$27, PeerJ_in_Computer_Science_Journ!K$39, Semantic_Web_Journal!K$20)</f>
         <v>15</v>
       </c>
-      <c r="J13" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K13" s="17">
+      <c r="J13" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K13" s="19">
         <f>SUM(Data_Science_Journal!K$28, PeerJ_in_Computer_Science_Journ!K$40, Semantic_Web_Journal!K$21)</f>
         <v>6</v>
       </c>
@@ -2605,7 +2614,7 @@
         <f t="shared" si="8"/>
         <v>3.404761905</v>
       </c>
-      <c r="M13" s="35">
+      <c r="M13" s="40">
         <f>MEDIAN(Data_Science_Journal!K$2:K$22,PeerJ_in_Computer_Science_Journ!K$2:K$33,Semantic_Web_Journal!K$2:K$15)</f>
         <v>3.5</v>
       </c>
@@ -2613,7 +2622,7 @@
         <f>STDEV(Data_Science_Journal!K$2:K$22,PeerJ_in_Computer_Science_Journ!K$2:K$33,Semantic_Web_Journal!K$2:K$15)</f>
         <v>1.037340027</v>
       </c>
-      <c r="O13" s="19">
+      <c r="O13" s="21">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
@@ -2625,55 +2634,55 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R13" s="36">
+      <c r="R13" s="22">
         <f t="shared" si="12"/>
         <v>0.0002715392343</v>
       </c>
-      <c r="S13" s="36">
+      <c r="S13" s="22">
         <f t="shared" si="13"/>
         <v>0.9999656144</v>
       </c>
-      <c r="T13" s="20">
+      <c r="T13" s="23">
         <f t="shared" si="14"/>
         <v>0.0001357696171</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="17">
         <v>1.0</v>
       </c>
       <c r="C14" s="6">
         <f>SUM(Data_Science_Journal!L$24, PeerJ_in_Computer_Science_Journ!L$36, Semantic_Web_Journal!L$17)</f>
         <v>2</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="17">
         <v>2.0</v>
       </c>
       <c r="E14" s="6">
         <f>SUM(Data_Science_Journal!L$25, PeerJ_in_Computer_Science_Journ!L$37, Semantic_Web_Journal!L$18)</f>
         <v>12</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="17">
         <v>3.0</v>
       </c>
       <c r="G14" s="6">
         <f>SUM(Data_Science_Journal!L$26, PeerJ_in_Computer_Science_Journ!L$38, Semantic_Web_Journal!L$19)</f>
         <v>8</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="17">
         <v>4.0</v>
       </c>
       <c r="I14" s="6">
         <f>SUM(Data_Science_Journal!L$27, PeerJ_in_Computer_Science_Journ!L$39, Semantic_Web_Journal!L$20)</f>
         <v>13</v>
       </c>
-      <c r="J14" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K14" s="17">
+      <c r="J14" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K14" s="19">
         <f>SUM(Data_Science_Journal!L$28, PeerJ_in_Computer_Science_Journ!L$40, Semantic_Web_Journal!L$21)</f>
         <v>7</v>
       </c>
@@ -2681,7 +2690,7 @@
         <f t="shared" si="8"/>
         <v>3.261904762</v>
       </c>
-      <c r="M14" s="35">
+      <c r="M14" s="40">
         <f>MEDIAN(Data_Science_Journal!L$2:L$22,PeerJ_in_Computer_Science_Journ!L$2:L$33,Semantic_Web_Journal!L$2:L$15)</f>
         <v>3</v>
       </c>
@@ -2689,7 +2698,7 @@
         <f>STDEV(Data_Science_Journal!L$2:L$22,PeerJ_in_Computer_Science_Journ!L$2:L$33,Semantic_Web_Journal!L$2:L$15)</f>
         <v>1.190603942</v>
       </c>
-      <c r="O14" s="19">
+      <c r="O14" s="21">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
@@ -2701,55 +2710,55 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R14" s="36">
+      <c r="R14" s="22">
         <f t="shared" si="12"/>
         <v>0.04355852192</v>
       </c>
-      <c r="S14" s="36">
+      <c r="S14" s="22">
         <f t="shared" si="13"/>
         <v>0.9902397636</v>
       </c>
-      <c r="T14" s="20">
+      <c r="T14" s="23">
         <f t="shared" si="14"/>
         <v>0.02177926096</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="17">
         <v>1.0</v>
       </c>
       <c r="C15" s="6">
         <f>SUM(Data_Science_Journal!M$24, PeerJ_in_Computer_Science_Journ!M$36, Semantic_Web_Journal!M$17)</f>
         <v>5</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="17">
         <v>2.0</v>
       </c>
       <c r="E15" s="6">
         <f>SUM(Data_Science_Journal!M$25, PeerJ_in_Computer_Science_Journ!M$37, Semantic_Web_Journal!M$18)</f>
         <v>4</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="17">
         <v>3.0</v>
       </c>
       <c r="G15" s="6">
         <f>SUM(Data_Science_Journal!M$26, PeerJ_in_Computer_Science_Journ!M$38, Semantic_Web_Journal!M$19)</f>
         <v>15</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="17">
         <v>4.0</v>
       </c>
       <c r="I15" s="6">
         <f>SUM(Data_Science_Journal!M$27, PeerJ_in_Computer_Science_Journ!M$39, Semantic_Web_Journal!M$20)</f>
         <v>13</v>
       </c>
-      <c r="J15" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K15" s="17">
+      <c r="J15" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K15" s="19">
         <f>SUM(Data_Science_Journal!M$28, PeerJ_in_Computer_Science_Journ!M$40, Semantic_Web_Journal!M$21)</f>
         <v>5</v>
       </c>
@@ -2757,7 +2766,7 @@
         <f t="shared" si="8"/>
         <v>3.214285714</v>
       </c>
-      <c r="M15" s="35">
+      <c r="M15" s="40">
         <f>MEDIAN(Data_Science_Journal!M$2:M$22,PeerJ_in_Computer_Science_Journ!M$2:M$33,Semantic_Web_Journal!M$2:M$15)</f>
         <v>3</v>
       </c>
@@ -2765,7 +2774,7 @@
         <f>STDEV(Data_Science_Journal!M$2:M$22,PeerJ_in_Computer_Science_Journ!M$2:M$33,Semantic_Web_Journal!M$2:M$15)</f>
         <v>1.158967461</v>
       </c>
-      <c r="O15" s="19">
+      <c r="O15" s="21">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
@@ -2777,55 +2786,55 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R15" s="36">
+      <c r="R15" s="22">
         <f t="shared" si="12"/>
         <v>0.0002715392343</v>
       </c>
-      <c r="S15" s="36">
+      <c r="S15" s="22">
         <f t="shared" si="13"/>
         <v>0.9999656144</v>
       </c>
-      <c r="T15" s="20">
+      <c r="T15" s="23">
         <f t="shared" si="14"/>
         <v>0.0001357696171</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="17">
         <v>1.0</v>
       </c>
       <c r="C16" s="6">
         <f>SUM(Data_Science_Journal!N$24, PeerJ_in_Computer_Science_Journ!N$36, Semantic_Web_Journal!N$17)</f>
         <v>2</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="17">
         <v>2.0</v>
       </c>
       <c r="E16" s="6">
         <f>SUM(Data_Science_Journal!N$25, PeerJ_in_Computer_Science_Journ!N$37, Semantic_Web_Journal!N$18)</f>
         <v>6</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="17">
         <v>3.0</v>
       </c>
       <c r="G16" s="6">
         <f>SUM(Data_Science_Journal!N$26, PeerJ_in_Computer_Science_Journ!N$38, Semantic_Web_Journal!N$19)</f>
         <v>12</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="17">
         <v>4.0</v>
       </c>
       <c r="I16" s="6">
         <f>SUM(Data_Science_Journal!N$27, PeerJ_in_Computer_Science_Journ!N$39, Semantic_Web_Journal!N$20)</f>
         <v>16</v>
       </c>
-      <c r="J16" s="15">
-        <v>5.0</v>
-      </c>
-      <c r="K16" s="17">
+      <c r="J16" s="17">
+        <v>5.0</v>
+      </c>
+      <c r="K16" s="19">
         <f>SUM(Data_Science_Journal!N$28, PeerJ_in_Computer_Science_Journ!N$40, Semantic_Web_Journal!N$21)</f>
         <v>6</v>
       </c>
@@ -2833,11 +2842,11 @@
         <f t="shared" si="8"/>
         <v>3.428571429</v>
       </c>
-      <c r="M16" s="35">
+      <c r="M16" s="40">
         <f>MEDIAN(Data_Science_Journal!N$2:N$22,PeerJ_in_Computer_Science_Journ!N$2:N$33,Semantic_Web_Journal!N$2:N$15)</f>
         <v>4</v>
       </c>
-      <c r="N16" s="37">
+      <c r="N16" s="41">
         <f>STDEV(Data_Science_Journal!N$2:N$22,PeerJ_in_Computer_Science_Journ!N$2:N$33,Semantic_Web_Journal!N$2:N$15)</f>
         <v>1.062506405</v>
       </c>
@@ -2853,91 +2862,91 @@
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R16" s="36">
+      <c r="R16" s="22">
         <f t="shared" si="12"/>
         <v>0.00006877111491</v>
       </c>
-      <c r="S16" s="36">
+      <c r="S16" s="22">
         <f t="shared" si="13"/>
         <v>0.9999924514</v>
       </c>
-      <c r="T16" s="20">
+      <c r="T16" s="23">
         <f t="shared" si="14"/>
         <v>0.00003438555746</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="25">
         <v>1.0</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="26">
         <f>SUM(Data_Science_Journal!O$24, PeerJ_in_Computer_Science_Journ!O$36, Semantic_Web_Journal!O$17)</f>
         <v>2</v>
       </c>
-      <c r="D17" s="22">
-        <v>2.0</v>
-      </c>
-      <c r="E17" s="23">
+      <c r="D17" s="25">
+        <v>2.0</v>
+      </c>
+      <c r="E17" s="26">
         <f>SUM(Data_Science_Journal!O$25, PeerJ_in_Computer_Science_Journ!O$37, Semantic_Web_Journal!O$18)</f>
         <v>3</v>
       </c>
-      <c r="F17" s="22">
-        <v>3.0</v>
-      </c>
-      <c r="G17" s="23">
+      <c r="F17" s="25">
+        <v>3.0</v>
+      </c>
+      <c r="G17" s="26">
         <f>SUM(Data_Science_Journal!O$26, PeerJ_in_Computer_Science_Journ!O$38, Semantic_Web_Journal!O$19)</f>
         <v>12</v>
       </c>
-      <c r="H17" s="22">
-        <v>4.0</v>
-      </c>
-      <c r="I17" s="23">
+      <c r="H17" s="25">
+        <v>4.0</v>
+      </c>
+      <c r="I17" s="26">
         <f>SUM(Data_Science_Journal!O$27, PeerJ_in_Computer_Science_Journ!O$39, Semantic_Web_Journal!O$20)</f>
         <v>17</v>
       </c>
-      <c r="J17" s="22">
-        <v>5.0</v>
-      </c>
-      <c r="K17" s="24">
+      <c r="J17" s="25">
+        <v>5.0</v>
+      </c>
+      <c r="K17" s="27">
         <f>SUM(Data_Science_Journal!O$28, PeerJ_in_Computer_Science_Journ!O$40, Semantic_Web_Journal!O$21)</f>
         <v>8</v>
       </c>
-      <c r="L17" s="25">
+      <c r="L17" s="28">
         <f t="shared" si="8"/>
         <v>3.619047619</v>
       </c>
-      <c r="M17" s="38">
+      <c r="M17" s="42">
         <f>MEDIAN(Data_Science_Journal!O$2:O$22,PeerJ_in_Computer_Science_Journ!O$2:O$33,Semantic_Web_Journal!O$2:O$15)</f>
         <v>4</v>
       </c>
-      <c r="N17" s="27">
+      <c r="N17" s="30">
         <f>STDEV(Data_Science_Journal!O$2:O$22,PeerJ_in_Computer_Science_Journ!O$2:O$33,Semantic_Web_Journal!O$2:O$15)</f>
         <v>1.034817787</v>
       </c>
-      <c r="O17" s="28">
+      <c r="O17" s="31">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="P17" s="25">
+      <c r="P17" s="28">
         <f t="shared" si="10"/>
         <v>37</v>
       </c>
-      <c r="Q17" s="25">
+      <c r="Q17" s="28">
         <f t="shared" si="11"/>
         <v>42</v>
       </c>
-      <c r="R17" s="39">
+      <c r="R17" s="32">
         <f t="shared" si="12"/>
         <v>0.0000004433704817</v>
       </c>
-      <c r="S17" s="39">
+      <c r="S17" s="32">
         <f t="shared" si="13"/>
         <v>0.9999999717</v>
       </c>
-      <c r="T17" s="29">
+      <c r="T17" s="33">
         <f t="shared" si="14"/>
         <v>0.0000002216852408</v>
       </c>
@@ -2971,7 +2980,7 @@
     <row r="20">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="40"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3156,7 +3165,7 @@
         <v>5.0</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -3206,10 +3215,10 @@
         <v>4.0</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -3259,7 +3268,7 @@
         <v>3.0</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -3309,10 +3318,10 @@
         <v>4.0</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -3362,10 +3371,10 @@
         <v>1.0</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
@@ -3415,10 +3424,10 @@
         <v>4.0</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -3468,7 +3477,7 @@
         <v>4.0</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -3571,7 +3580,7 @@
         <v>5.0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
@@ -3621,7 +3630,7 @@
         <v>4.0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23">
@@ -4119,10 +4128,10 @@
         <v>4.0</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -4172,10 +4181,10 @@
         <v>2.0</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -4225,7 +4234,7 @@
         <v>3.0</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -4275,7 +4284,7 @@
         <v>4.0</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -4325,7 +4334,7 @@
         <v>5.0</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
@@ -4375,10 +4384,10 @@
         <v>3.0</v>
       </c>
       <c r="P8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q8" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -4481,7 +4490,7 @@
         <v>5.0</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -4531,10 +4540,10 @@
         <v>2.0</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -4584,7 +4593,7 @@
         <v>3.0</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13">
@@ -4937,7 +4946,7 @@
         <v>4.0</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20">

</xml_diff>